<commit_message>
added email formatting and fix minor bugs
</commit_message>
<xml_diff>
--- a/src/config.xlsx
+++ b/src/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\PycharmProjects\memgpt\auto_mailer\Auto-Mailer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\PycharmProjects\memgpt\auto_mailer\Auto-Mailer\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DB5A43-9827-4DF7-99CD-EC24DFAAEDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976AD519-8063-4969-B472-F61A18C0B3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emails" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
@@ -40,15 +40,6 @@
     <t>amityadav4664@gmail.com</t>
   </si>
   <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>Hi this is test email to all users belonging to group 1</t>
-  </si>
-  <si>
-    <t>Hi this is test email to all users belonging to group 2</t>
-  </si>
-  <si>
     <t>attachment</t>
   </si>
   <si>
@@ -58,15 +49,6 @@
     <t>subject</t>
   </si>
   <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>test123@outlook.com</t>
-  </si>
-  <si>
-    <t>Auto Mailer Test Email</t>
-  </si>
-  <si>
     <t>Auto Mailer Test Email 2</t>
   </si>
   <si>
@@ -74,6 +56,12 @@
   </si>
   <si>
     <t>report2</t>
+  </si>
+  <si>
+    <t>formatted outlook email</t>
+  </si>
+  <si>
+    <t>shweta.pawar8652@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -404,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +420,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -440,40 +428,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F1BA5E33-5876-4D04-BDA4-4B50C33C2480}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{F9F7E5B8-DB38-4618-9BF0-59D43DD2E64E}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{CDDD50EC-BE30-4A5D-A096-3AD34B6F7145}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{71BD101E-725E-43E9-98B5-DE93E75511BC}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{AB27BD52-FB98-4E8C-967C-05E5647BCF85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -493,55 +463,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5F2174-BEFD-4FBD-82E1-2EB6F01ACF81}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated script to support cc and bcc in email
</commit_message>
<xml_diff>
--- a/src/config.xlsx
+++ b/src/config.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\PycharmProjects\memgpt\auto_mailer\Auto-Mailer\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976AD519-8063-4969-B472-F61A18C0B3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97499EAD-F24C-441F-A7DA-58FF02992B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="emails" sheetId="1" r:id="rId1"/>
-    <sheet name="messages" sheetId="2" r:id="rId2"/>
+    <sheet name="messages" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>group_id</t>
   </si>
@@ -61,7 +54,22 @@
     <t>formatted outlook email</t>
   </si>
   <si>
-    <t>shweta.pawar8652@gmail.com</t>
+    <t>send_email_to</t>
+  </si>
+  <si>
+    <t>send_email_cc</t>
+  </si>
+  <si>
+    <t>send_email_bcc</t>
+  </si>
+  <si>
+    <t>amityadav4664@gmail.com;test@gmail.com;test123@gmail.com</t>
+  </si>
+  <si>
+    <t>C:\Users\Amit\Downloads\b.jpeg;C:\Users\Amit\Downloads\a.jpeg;</t>
+  </si>
+  <si>
+    <t>test456@gmail.com;test321@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -106,9 +114,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -389,84 +405,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F1BA5E33-5876-4D04-BDA4-4B50C33C2480}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{AB27BD52-FB98-4E8C-967C-05E5647BCF85}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{43BBC384-92DC-4E22-9957-F24935033511}">
-          <x14:formula1>
-            <xm:f>messages!$A$2:$A$1048576</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5F2174-BEFD-4FBD-82E1-2EB6F01ACF81}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,42 +417,496 @@
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{14134550-6699-4853-92F6-3A3FF03AAF30}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{71B88399-D42D-4401-B064-B08AD7244E24}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{A3132E7F-2BD9-4525-A27D-E2E6CA41ED6C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>